<commit_message>
the script now suports multidimentional linear regression
</commit_message>
<xml_diff>
--- a/points.xlsx
+++ b/points.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohamadhoseyn/Desktop/Programs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohamadhoseyn/Desktop/Programs/regression/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7CD786-364A-9544-B810-ABDF80657DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D04C86D-8FB7-A640-82CB-7BFD1570F321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="17320" windowHeight="15060" xr2:uid="{D60F6389-8449-824D-AECA-EF7860BF85FD}"/>
   </bookViews>
@@ -36,12 +36,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>temp</t>
   </si>
   <si>
     <t>wind_speed</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>21`</t>
   </si>
 </sst>
 </file>
@@ -413,260 +419,353 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC1C4655-1780-3B4F-9E89-B88E27C92A79}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>14.6</v>
       </c>
       <c r="B2">
         <v>18.600000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>7</v>
       </c>
       <c r="B3">
         <v>13.6</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>20.7</v>
       </c>
       <c r="B4">
         <v>21.8</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>25.3</v>
       </c>
       <c r="B5">
         <v>20.8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>14.6</v>
       </c>
       <c r="B6">
         <v>17.8</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>23.4</v>
       </c>
       <c r="B7">
         <v>15.1</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>25.6</v>
       </c>
       <c r="B8">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>14.9</v>
       </c>
       <c r="B9">
         <v>24.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>26.8</v>
       </c>
       <c r="B10">
         <v>14.1</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>11.8</v>
       </c>
       <c r="B11">
         <v>13.4</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>18</v>
       </c>
       <c r="B12">
         <v>21.6</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>19.6666666666667</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10.8</v>
       </c>
       <c r="B13">
         <v>13.7</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>22.1666666666667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>20.7</v>
       </c>
       <c r="B14">
         <v>18.7</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <v>24.6666666666667</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>6.5</v>
       </c>
       <c r="B15">
         <v>10.6</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <v>27.1666666666667</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>9</v>
       </c>
       <c r="B16">
         <v>19.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>29.6666666666667</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>25.8</v>
       </c>
       <c r="B17">
         <v>15.1</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>26.1</v>
       </c>
       <c r="B18">
         <v>32.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>5.6</v>
       </c>
       <c r="B19">
         <v>14.6</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>15.8</v>
       </c>
       <c r="B20">
         <v>13.3</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>9.8000000000000007</v>
       </c>
       <c r="B21">
         <v>7.7</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>24.1</v>
       </c>
       <c r="B22">
         <v>25.2</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>9.4</v>
       </c>
       <c r="B23">
         <v>19.399999999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>9.8000000000000007</v>
       </c>
       <c r="B24">
         <v>14.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23.8</v>
       </c>
       <c r="B25">
         <v>20.2</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>20.399999999999999</v>
       </c>
       <c r="B26">
         <v>38.299999999999997</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>18.100000000000001</v>
       </c>
       <c r="B27">
         <v>24.4</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>25.4</v>
       </c>
       <c r="B28">
         <v>23</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>16.2</v>
       </c>
       <c r="B29">
         <v>17.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>9.1</v>
       </c>
       <c r="B30">
         <v>16.100000000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>8.1</v>
       </c>
       <c r="B31">
         <v>15.1</v>
+      </c>
+      <c r="C31">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>